<commit_message>
210513_mapper 기능 1차 작업 완료
</commit_message>
<xml_diff>
--- a/서버관련자료/mapper기능정리.xlsx
+++ b/서버관련자료/mapper기능정리.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="300">
   <si>
     <t>default sysdate</t>
   </si>
@@ -531,22 +531,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>d, name, email</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>id, name, email 검색 -&gt; passwd 수정 -&gt; 1(수정) 0(수정불가) 반환</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -606,10 +590,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>email, passwd 검색 -&gt; 정보 삭제 -&gt; 1(수정) 0(수정불가) 반환</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>rank, reserves, totalprice, birth</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -630,10 +610,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>rank, reserves, totalprice, birth -&gt; 검색 -&gt; 해당회원리스트 출력</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>m</t>
     </r>
@@ -662,22 +638,6 @@
         <charset val="129"/>
       </rPr>
       <t xml:space="preserve"> 앱 관련 정보 제공</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>eserves</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -748,23 +708,630 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>리뷰수</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>review</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>comscore</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글 수</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>VARCHAR(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>50)</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>u</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>rl 형식으로 저장</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>reviewscore</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>장바구니</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cartnum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원장바구니삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>d, name, email</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, order_result(1)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, prodnum, quantity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니합계</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, order_result(1)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>list</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rank, reserves, totalprice, birth 검색 -&gt; 해당회원리스트 출력</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, order_result(1) 검색 -&gt; 구입예정 제품 리스트 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cartnum 검색 -&gt; 1(삭제완료) 0(삭제불가-서버에러 등)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email 검색 -&gt; 1(삭제완료) 0(삭제불가-서버에러 등)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, passwd 매칭 검색 -&gt; 정보 삭제 -&gt; 1(수정) 0(수정불가) 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">email 검색 -&gt; prodnum, quantity 추가 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>-&gt; 1(추가) 0(불가-서버에러등)</t>
+  </si>
+  <si>
+    <t>email, order_result(1) 검색 -&gt; prodnum*quantity 값 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문목록</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송전</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송중</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송완료</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>적립금조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>적립금조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품이미지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, order_detail_state(2)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>eserves</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email 검색 -&gt; 적립금(reserves) 조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>prodnum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>prodnum 검색 -&gt; url 주소로 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ordernum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ordernum검색 -&gt; 1(삭제완료) 0(삭제불가-서버에러 등)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>prodnum 검색 -&gt; 상품 정보 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품목록</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>rod 테이블</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 목록 제공</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품등록</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>name, kind, price, content</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>detail, image</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>필수항목과 나머지 항목에 대한 데이터 체크하여 DB에 저장</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>prodnum, name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>prodnum,. Name 검색 -&gt; price, content, detail, image 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; 1(수정완료) 2(수정불가-서버에러 등)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>등급별조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품재고</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stock</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">defalut </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, order_detail_result(2)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, order_detail_result(3)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, order_detail_result(3) 검색 -&gt; 배송완료 리스트 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, order_detail_result(2) 검색 -&gt; 배송중 목록 리스트 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, state, result 검색 -&gt; 주문완료 -&gt; 상품목록 리스트 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, order_detail_state(2) 검색 -&gt; 구입완료 목록 리스트 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, order_detail_state(2)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, state, result 검색 -&gt; 주문완료 -&gt; 적립금 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email 검색 -&gt; 적립금 조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email 검색 -&gt; 등급별 조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>prodnum, name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>prodnum, name 검색 -&gt; 재고 수량 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>리뷰수</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>review</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>comscore</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>댓글 수</t>
+    <t>prodnum,. Name 검색 -&gt; 리뷰 수 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰점수</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>prodnum,. Name 검색 -&gt; 리뷰 점수 평균 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품별 리뷰 목록</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원별 리뷰 목록</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>prodnum 검색 -&gt; renum, email, rename, lookup, recom, comscore,</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>grade 등  필요한 리스트 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email 검색 -&gt; renum, prodnum, rename, lookup, recom, comscore,</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>renum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>renum, rename</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>renum, rename(대부분 제목클릭) 검색 -&gt; 리뷰 리스트 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰 삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰 조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">renum 검색 -&gt; rename, content, grade 수정 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>renum 검색 -&gt; 리뷰 삭제 -&gt; 1(삭제완료) 2(삭제불가) 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>prodnum,. Name 검색 -&gt; 상품 삭제 -&gt; 1(삭제완료) 2(삭제불가) 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>1(수정) 0(수정불가) 반환</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 정보 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 정보 조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>adminmember 테이블</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>adminmember_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>adminmember_id 검색 -&gt; 수정 -&gt; 1(수정) 0(수정불가) 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지 목록 조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지 조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지 삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>notice 테이블</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>notic 테이블 목록 조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>notinum, name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>notinum, name(대부분 제목클릭) 검색 -&gt; 공지 리스트 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>notinum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>notinum 검색 -&gt; 공지 삭제 -&gt; 1(삭제완료) 2(삭제불가) 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>notinum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>notinum 검색 -&gt; name, content 수정 -&gt; 1(수정) 0(수정불가) 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qna 목록 조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qna 조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qna 삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qna 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qna 테이블</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qnanum, name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qnanum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qnanum 검색 -&gt; name, content 수정 -&gt; 1(수정) 0(수정불가) 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qna 테이블 목록 조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qnanum, name(대부분 제목클릭) 검색 -&gt; qna 리스트 반환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qnanum 검색 -&gt; qna 삭제 -&gt; 1(삭제완료) 2(삭제불가) 반환</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -826,7 +1393,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -888,13 +1455,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -964,7 +1549,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1433,24 +2057,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:M109"/>
+  <dimension ref="B2:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="I88" sqref="I88"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.375" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="39.375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.125" customWidth="1"/>
-    <col min="9" max="9" width="13.125" customWidth="1"/>
-    <col min="10" max="10" width="25.75" customWidth="1"/>
-    <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="12" max="12" width="55.875" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="38.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.875" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="28.875" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="60.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
@@ -1461,10 +2085,10 @@
         <v>16</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="I2" s="13"/>
+      <c r="I2" s="24"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -1526,7 +2150,7 @@
         <v>147</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
@@ -1582,7 +2206,7 @@
         <v>152</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
@@ -1608,13 +2232,13 @@
         <v>141</v>
       </c>
       <c r="J7" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="L7" s="20" t="s">
         <v>153</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="L7" s="20" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
@@ -1637,16 +2261,16 @@
         <v>5</v>
       </c>
       <c r="I8" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="J8" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="K8" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="L8" s="22" t="s">
         <v>159</v>
-      </c>
-      <c r="L8" s="22" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
@@ -1670,7 +2294,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
@@ -1694,13 +2318,13 @@
         <v>143</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
@@ -1722,13 +2346,13 @@
         <v>144</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
@@ -1745,39 +2369,23 @@
       <c r="F12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="4">
-        <v>8</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>168</v>
-      </c>
     </row>
     <row r="13" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="17" t="s">
-        <v>169</v>
+        <v>210</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+      <c r="H13" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="I13" s="24"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
@@ -1793,11 +2401,21 @@
       <c r="F14" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
+      <c r="H14" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>138</v>
+      </c>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
@@ -1814,20 +2432,40 @@
       <c r="F15" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
+      <c r="H15" s="4">
+        <v>1</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="K15" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>193</v>
+      </c>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E16" s="2"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
+      <c r="H16" s="4">
+        <v>2</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="J16" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="K16" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>194</v>
+      </c>
       <c r="M16" s="6"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
@@ -1838,11 +2476,21 @@
         <v>46</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
+      <c r="H17" s="4">
+        <v>3</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="K17" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="L17" s="19" t="s">
+        <v>195</v>
+      </c>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
@@ -1861,11 +2509,21 @@
       <c r="F18" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
+      <c r="H18" s="21">
+        <v>4</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="K18" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="L18" s="25" t="s">
+        <v>197</v>
+      </c>
       <c r="M18" s="6"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
@@ -1884,11 +2542,13 @@
       <c r="F19" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="8"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10" t="s">
+        <v>198</v>
+      </c>
       <c r="M19" s="6"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
@@ -1907,6 +2567,21 @@
       <c r="F20" s="4" t="s">
         <v>115</v>
       </c>
+      <c r="H20" s="4">
+        <v>5</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
@@ -1924,6 +2599,11 @@
       <c r="F21" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="27"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
@@ -1939,6 +2619,13 @@
         <v>107</v>
       </c>
       <c r="F22" s="4"/>
+      <c r="H22" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="I22" s="28"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
@@ -1952,6 +2639,21 @@
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
+      <c r="H23" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
@@ -1965,9 +2667,39 @@
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
+      <c r="H24" s="21">
+        <v>1</v>
+      </c>
+      <c r="I24" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="K24" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="L24" s="22" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E25" s="2"/>
+      <c r="H25" s="4">
+        <v>2</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="K25" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="L25" s="19" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="13" t="s">
@@ -1977,6 +2709,21 @@
         <v>31</v>
       </c>
       <c r="E26" s="2"/>
+      <c r="H26" s="4">
+        <v>3</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="K26" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="L26" s="19" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="11" t="s">
@@ -1994,6 +2741,21 @@
       <c r="F27" s="11" t="s">
         <v>119</v>
       </c>
+      <c r="H27" s="4">
+        <v>4</v>
+      </c>
+      <c r="I27" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="K27" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="4" t="s">
@@ -2009,6 +2771,21 @@
       <c r="F28" s="3" t="s">
         <v>98</v>
       </c>
+      <c r="H28" s="34">
+        <v>5</v>
+      </c>
+      <c r="I28" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="J28" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="L28" s="17" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
@@ -2037,6 +2814,13 @@
       <c r="F30" s="4" t="s">
         <v>86</v>
       </c>
+      <c r="H30" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="I30" s="23"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
@@ -2050,6 +2834,21 @@
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
+      <c r="H31" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J31" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="L31" s="16" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
@@ -2063,49 +2862,105 @@
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H32" s="4">
+        <v>1</v>
+      </c>
+      <c r="I32" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="J32" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="K32" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="L32" s="29" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="C33" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H33" s="4">
         <v>2</v>
       </c>
-      <c r="D33" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I33" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="J33" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="K33" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="L33" s="17" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F34" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H34" s="21">
+        <v>3</v>
+      </c>
+      <c r="I34" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="J34" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="K34" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="L34" s="22" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="17" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="K35" s="2"/>
+      <c r="L35" s="10"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="17" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>94</v>
@@ -2117,930 +2972,1478 @@
       <c r="F36" s="4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" s="4" t="s">
+      <c r="H36" s="21">
+        <v>4</v>
+      </c>
+      <c r="I36" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="J36" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="K36" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="L36" s="22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="H37" s="10"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="33" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B38" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4" t="s">
+      <c r="E38" s="4"/>
+      <c r="F38" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B38" s="4" t="s">
+      <c r="H38" s="4">
+        <v>5</v>
+      </c>
+      <c r="I38" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="J38" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="K38" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="L38" s="17" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B39" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" s="13" t="s">
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="H39" s="34">
+        <v>6</v>
+      </c>
+      <c r="I39" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="J39" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="L39" s="17" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E40" s="2"/>
+      <c r="H40" s="34">
+        <v>7</v>
+      </c>
+      <c r="I40" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="J40" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="K40" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="L40" s="17" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B41" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C41" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" s="11" t="s">
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B42" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C42" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D42" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E42" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F42" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="4" t="s">
+      <c r="H42" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="I42" s="28"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B43" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>122</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F43" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J43" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="K43" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="L43" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B44" s="4" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="H44" s="4">
+        <v>1</v>
+      </c>
+      <c r="I44" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="J44" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="K44" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L44" s="17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B45" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="H45" s="4">
+        <v>2</v>
+      </c>
+      <c r="I45" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="J45" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="K45" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L45" s="17" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B46" s="4" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F46" s="4"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F46" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H46" s="4">
+        <v>3</v>
+      </c>
+      <c r="I46" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="J46" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="K46" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L46" s="17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B47" s="4" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F47" s="4"/>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H47" s="34">
+        <v>4</v>
+      </c>
+      <c r="I47" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="J47" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="K47" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="L47" s="17" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B48" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F48" s="4"/>
+      <c r="H48" s="34">
+        <v>5</v>
+      </c>
+      <c r="I48" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="J48" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="K48" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L48" s="17" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B49" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C49" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D49" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4" t="s">
+      <c r="E49" s="4"/>
+      <c r="F49" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E49" s="2"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B50" s="13" t="s">
+      <c r="H49" s="4">
+        <v>6</v>
+      </c>
+      <c r="I49" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="J49" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="K49" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="L49" s="17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E50" s="2"/>
+      <c r="H50" s="34">
+        <v>7</v>
+      </c>
+      <c r="I50" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="J50" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="K50" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="L50" s="32" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B51" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C51" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B51" s="11" t="s">
+      <c r="E51" s="2"/>
+      <c r="H51" s="34">
+        <v>8</v>
+      </c>
+      <c r="I51" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="J51" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="K51" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L51" s="32" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B52" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C52" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D52" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E52" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F51" s="11" t="s">
+      <c r="F52" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B52" s="4" t="s">
+      <c r="H52" s="34">
+        <v>9</v>
+      </c>
+      <c r="I52" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="J52" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="K52" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="L52" s="32" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B53" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B53" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>122</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F53" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F53" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B54" s="4" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>122</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="H54" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="I54" s="28"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B55" s="4" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="I55" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J55" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="K55" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="L55" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B56" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="H56" s="21">
+        <v>1</v>
+      </c>
+      <c r="I56" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="J56" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="K56" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="L56" s="22" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B57" s="4" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F57" s="4"/>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="19"/>
+      <c r="L57" s="19" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B58" s="4" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F58" s="4"/>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H58" s="21">
+        <v>2</v>
+      </c>
+      <c r="I58" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="J58" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="K58" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="L58" s="22" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B59" s="4" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>122</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E59" s="4"/>
+        <v>76</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="F59" s="4"/>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H59" s="10"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="19"/>
+      <c r="K59" s="19"/>
+      <c r="L59" s="19" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B60" s="4" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>122</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H60" s="4">
+        <v>3</v>
+      </c>
+      <c r="I60" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="J60" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="K60" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="L60" s="17" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B61" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="H61" s="34">
+        <v>4</v>
+      </c>
+      <c r="I61" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="J61" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="K61" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="L61" s="17" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B62" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C62" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D62" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B62" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="H62" s="35">
+        <v>5</v>
+      </c>
+      <c r="I62" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="J62" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="K62" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="L62" s="22" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B63" s="4" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>99</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H63" s="10"/>
+      <c r="I63" s="30"/>
+      <c r="J63" s="10"/>
+      <c r="K63" s="10"/>
+      <c r="L63" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B64" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B64" s="4" t="s">
+      <c r="H64" s="26"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B65" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C65" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D65" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B65" s="6"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
-      <c r="E65" s="6"/>
-      <c r="F65" s="6"/>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B66" s="13" t="s">
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="H65" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="I65" s="28"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="H66" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="I66" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J66" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="K66" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="L66" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B67" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C66" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="E66" s="2"/>
-    </row>
-    <row r="67" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="11" t="s">
+      <c r="C67" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="E67" s="2"/>
+      <c r="H67" s="4">
+        <v>1</v>
+      </c>
+      <c r="I67" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="J67" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="K67" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L67" s="17" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C68" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="D68" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E67" s="12" t="s">
+      <c r="E68" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F67" s="11" t="s">
+      <c r="F68" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B68" s="4" t="s">
+      <c r="H68" s="4">
+        <v>2</v>
+      </c>
+      <c r="I68" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="J68" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="K68" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L68" s="17" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B69" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B69" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>122</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F69" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F69" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H69" s="4">
+        <v>3</v>
+      </c>
+      <c r="I69" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="J69" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="K69" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="L69" s="17" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B70" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="H70" s="34">
+        <v>4</v>
+      </c>
+      <c r="I70" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="J70" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="K70" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="L70" s="17" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B71" s="4" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F71" s="4"/>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F71" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H71" s="26"/>
+      <c r="I71" s="36"/>
+      <c r="J71" s="26"/>
+      <c r="K71" s="26"/>
+      <c r="L71" s="27" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B72" s="4" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F72" s="4"/>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H72" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="I72" s="28"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B73" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F73" s="4"/>
+      <c r="H73" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="I73" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J73" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="K73" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="L73" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B74" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B74" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>122</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H74" s="4">
+        <v>1</v>
+      </c>
+      <c r="I74" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="J74" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="K74" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L74" s="17" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B75" s="4" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>122</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B76" s="17" t="s">
-        <v>178</v>
+      <c r="H75" s="4">
+        <v>2</v>
+      </c>
+      <c r="I75" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="J75" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="K75" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L75" s="17" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B76" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D76" s="17" t="s">
-        <v>179</v>
+      <c r="D76" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B77" s="7" t="s">
+      <c r="H76" s="4">
+        <v>3</v>
+      </c>
+      <c r="I76" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="J76" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="K76" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="L76" s="17" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B77" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D77" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="H77" s="34">
+        <v>4</v>
+      </c>
+      <c r="I77" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="J77" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="K77" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="L77" s="17" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B78" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C78" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D78" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E77" s="4" t="s">
+      <c r="E78" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F77" s="4"/>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B78" s="4" t="s">
+      <c r="F78" s="4"/>
+      <c r="H78" s="26"/>
+      <c r="I78" s="26"/>
+      <c r="J78" s="26"/>
+      <c r="K78" s="26"/>
+      <c r="L78" s="26"/>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B79" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C79" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D79" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B79" s="6"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B80" s="13" t="s">
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="6"/>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="6"/>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B81" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C80" s="13" t="s">
+      <c r="C81" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="E80" s="2"/>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B81" s="11" t="s">
+      <c r="E81" s="2"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B82" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="C82" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D81" s="11" t="s">
+      <c r="D82" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E81" s="12" t="s">
+      <c r="E82" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F81" s="11" t="s">
+      <c r="F82" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B82" s="4" t="s">
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B83" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C83" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D82" s="4" t="s">
+      <c r="D83" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="E82" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B83" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F83" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F83" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B84" s="4" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>124</v>
+        <v>78</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F84" s="4"/>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F84" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B85" s="4" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F85" s="4"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B86" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F86" s="4"/>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B87" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C87" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="D87" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="E87" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F86" s="4"/>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B87" s="6"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="6"/>
-      <c r="F87" s="6"/>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B88" s="13" t="s">
+      <c r="F87" s="4"/>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B89" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C88" s="13" t="s">
+      <c r="C89" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E88" s="2"/>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B89" s="11" t="s">
+      <c r="E89" s="2"/>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B90" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C89" s="11" t="s">
+      <c r="C90" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D89" s="11" t="s">
+      <c r="D90" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E89" s="12" t="s">
+      <c r="E90" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F89" s="11" t="s">
+      <c r="F90" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B90" s="4" t="s">
+    <row r="91" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B91" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C91" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D90" s="4" t="s">
+      <c r="D91" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="E90" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B91" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F91" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F91" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B92" s="4" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="E92" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F92" s="4"/>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F92" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B93" s="4" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F93" s="4"/>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B94" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F94" s="4"/>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B95" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C95" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="D95" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="F94" s="4"/>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B95" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>132</v>
       </c>
       <c r="F95" s="4"/>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B96" s="6"/>
-      <c r="C96" s="6"/>
-      <c r="D96" s="6"/>
-      <c r="E96" s="6"/>
-      <c r="F96" s="6"/>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B96" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F96" s="4"/>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E97" s="2"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B98" s="13" t="s">
+      <c r="E98" s="2"/>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B99" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C98" s="13" t="s">
+      <c r="C99" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E98" s="2"/>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B99" s="11" t="s">
+      <c r="E99" s="2"/>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B100" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C99" s="11" t="s">
+      <c r="C100" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D99" s="11" t="s">
+      <c r="D100" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E99" s="12" t="s">
+      <c r="E100" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F99" s="11" t="s">
+      <c r="F100" s="11" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B100" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D100" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E100" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B101" s="4" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>105</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F101" s="3"/>
+      <c r="F101" s="3" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B102" s="4" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>105</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F102" s="4"/>
+      <c r="F102" s="3"/>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B103" s="4" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>107</v>
@@ -3049,13 +4452,13 @@
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B104" s="4" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>107</v>
@@ -3063,18 +4466,26 @@
       <c r="F104" s="4"/>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B105" s="6"/>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6"/>
-      <c r="F105" s="8"/>
+      <c r="B105" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F105" s="4"/>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
       <c r="D106" s="6"/>
       <c r="E106" s="6"/>
-      <c r="F106" s="6"/>
+      <c r="F106" s="8"/>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B107" s="6"/>
@@ -3097,7 +4508,19 @@
       <c r="E109" s="6"/>
       <c r="F109" s="6"/>
     </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51138889789581299" footer="0.51138889789581299"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>